<commit_message>
Mirrored inputs from ts_config in ExcelParser and xslx
</commit_message>
<xml_diff>
--- a/ts_core/utils/ExcelParse/Configuration.xlsx
+++ b/ts_core/utils/ExcelParse/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan\Documents\MSD\trafficsensemsd\ExcelParse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan\Documents\MSD\trafficsensemsd\core\ts_core\utils\ExcelParse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Cross</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Intersection Shape</t>
   </si>
   <si>
@@ -77,13 +74,71 @@
   </si>
   <si>
     <t>Route Weights</t>
+  </si>
+  <si>
+    <t>Randomize</t>
+  </si>
+  <si>
+    <t>Don't Randomize</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Randomize                                         </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(slightly randomizes the configuration)</t>
+    </r>
+  </si>
+  <si>
+    <t>Size Distribution</t>
+  </si>
+  <si>
+    <t>V2I Distribution</t>
+  </si>
+  <si>
+    <t>Pre-Timed based on Historical Demand</t>
+  </si>
+  <si>
+    <t>Pre-Timed based on Historical Demand + Detection for interval extension/interruption</t>
+  </si>
+  <si>
+    <t>LSTM Network</t>
+  </si>
+  <si>
+    <t>Deep Q-Learning Network</t>
+  </si>
+  <si>
+    <t>User Supplied</t>
+  </si>
+  <si>
+    <t>Initialize the Directory</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Options List 2</t>
+  </si>
+  <si>
+    <t>Options List 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +168,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -176,13 +245,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -190,7 +271,10 @@
     <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -209,19 +293,21 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="2">
-    <queryTableFields count="1">
+  <queryTableRefresh nextId="3" unboundColumnsRight="1">
+    <queryTableFields count="2">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
+      <queryTableField id="2" dataBound="0" tableColumnId="2"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DF6379D-0736-4942-AE6F-4D162B1AE803}" name="Table1_2" displayName="Table1_2" ref="A14:A17" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A14:A17" xr:uid="{8663D33E-6A5B-42FF-B352-2AA5751D2CCE}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{07F52DF6-6FB4-4DB8-B5F4-646E8DCC4A98}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DF6379D-0736-4942-AE6F-4D162B1AE803}" name="Table1_2" displayName="Table1_2" ref="A14:B17" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A14:B17" xr:uid="{8663D33E-6A5B-42FF-B352-2AA5751D2CCE}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{07F52DF6-6FB4-4DB8-B5F4-646E8DCC4A98}" uniqueName="1" name="Options List 1" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{24EB9063-8E55-4D9F-9954-FD590EB32E9B}" uniqueName="2" name="Options List 2" queryTableFieldId="2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -525,87 +611,163 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06AEE040-40BA-4301-85DF-18947967B3AF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="6" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
     <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="F15" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4" xr:uid="{F042EE89-7603-4A9F-9A58-A60601344CCD}">
       <formula1>$A$15:$A$17</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A11" xr:uid="{EFE5F3E3-9DAC-478A-A1C0-9A719EE4ED18}">
+      <formula1>$A$20:$A$21</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{C4122F11-C831-4D9F-8AE9-607483206EEB}">
+      <formula1>$F$14:$F$18</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{32E14B11-4650-42FE-AA14-8539AD4081FB}">
+      <formula1>$B$16:$B$17</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>